<commit_message>
GDE-6965 Updated variables on test suite update validation keyword Updated data set with correct values for facility_type, facility_OwningBranch and payload_effectiveDate
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/SAPWUL/SAPWUL_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/SAPWUL/SAPWUL_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="353" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="565" firstSheet="1" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DealData" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -61,6 +61,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <color indexed="30"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0070C0"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -160,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -200,6 +212,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +526,7 @@
   <dimension ref="A1:BT12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:M4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -973,12 +987,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SAPCRE01_20022020090946GFZ</t>
+          <t>SAPCRE01_14092020151257QHW</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>D1_20022020090947JYF</t>
+          <t>D1_14092020151259VPE</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -4908,9 +4922,9 @@
   <dimension ref="A1:BI33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="AF1" activePane="topRight" state="frozen"/>
       <selection activeCell="B8" sqref="B8"/>
-      <selection pane="topRight" activeCell="N6" sqref="N6:Q6"/>
+      <selection pane="topRight" activeCell="AK7" sqref="AK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -5227,12 +5241,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SAPCRE01_20022020090946GFZ</t>
+          <t>SAPCRE01_14092020151257QHW</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FACILITY-A_20022020091648</t>
+          <t>FACILITY-A_14092020152142</t>
         </is>
       </c>
       <c r="I2" s="33" t="inlineStr">
@@ -7685,7 +7699,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AI12" s="7" t="inlineStr">
+      <c r="AI12" s="14" t="inlineStr">
         <is>
           <t>Agency Australia</t>
         </is>
@@ -7779,12 +7793,12 @@
       </c>
       <c r="G13" s="1" t="inlineStr">
         <is>
-          <t>SAPCRE01_20022020090946GFZ</t>
+          <t>SAPCRE01_14092020151257QHW</t>
         </is>
       </c>
       <c r="H13" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_20022020091648</t>
+          <t>FACILITY-A_14092020152142</t>
         </is>
       </c>
       <c r="I13" s="33" t="inlineStr">
@@ -7797,9 +7811,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K13" s="14" t="inlineStr">
-        <is>
-          <t>Revolver</t>
+      <c r="K13" s="36" t="inlineStr">
+        <is>
+          <t>Term</t>
         </is>
       </c>
       <c r="L13" s="15" t="inlineStr">
@@ -7907,9 +7921,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AG13" s="7" t="inlineStr">
-        <is>
-          <t>Commonwealth Bank of Australia - OBU</t>
+      <c r="AG13" s="35" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
       <c r="AH13" s="7" t="inlineStr">
@@ -8396,7 +8410,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AI15" s="7" t="inlineStr">
+      <c r="AI15" s="14" t="inlineStr">
         <is>
           <t>Non-Agency Australia</t>
         </is>
@@ -8490,12 +8504,12 @@
       </c>
       <c r="G16" s="1" t="inlineStr">
         <is>
-          <t>SAPCRE01_07102019090234GKV</t>
+          <t>SAPCRE01_11092020114456BLP</t>
         </is>
       </c>
       <c r="H16" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_07102019093752KLO</t>
+          <t>FACILITY-A_11092020115319</t>
         </is>
       </c>
       <c r="I16" s="33" t="inlineStr">
@@ -12726,7 +12740,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_20022020091648</t>
+          <t>FACILITY-A_14092020152142</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -13722,7 +13736,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection pane="topRight" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -13901,7 +13915,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FACILITY-A_20022020091648</t>
+          <t>FACILITY-A_14092020152142</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -13911,7 +13925,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3000046</t>
+          <t>3000663</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -13952,12 +13966,12 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>AZE5UHIL</t>
+          <t>WUEGI81M</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>RPTMGR01</t>
+          <t>MGRDEL01</t>
         </is>
       </c>
       <c r="U2" s="1" t="inlineStr">
@@ -14052,7 +14066,7 @@
           <t>true|true|true</t>
         </is>
       </c>
-      <c r="Q3" s="33" t="inlineStr"/>
+      <c r="Q3" s="33" t="n"/>
       <c r="R3" s="1" t="inlineStr">
         <is>
           <t>user|user|user</t>
@@ -14111,7 +14125,7 @@
         </is>
       </c>
       <c r="G4" s="7" t="n"/>
-      <c r="Q4" s="33" t="inlineStr"/>
+      <c r="Q4" s="33" t="n"/>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="34">
       <c r="A5" s="1" t="inlineStr">
@@ -14150,7 +14164,7 @@
           <t>2018-03-26</t>
         </is>
       </c>
-      <c r="Q5" s="33" t="inlineStr"/>
+      <c r="Q5" s="33" t="n"/>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="34">
       <c r="A6" s="1" t="inlineStr">
@@ -14427,22 +14441,22 @@
       </c>
       <c r="H9" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_07102019093752KLO</t>
+          <t>FACILITY-A_14092020152142</t>
         </is>
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>RST</t>
+          <t>TAM</t>
         </is>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>03000160</t>
+          <t>3000663</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr">
         <is>
-          <t>CB022</t>
+          <t>CB001</t>
         </is>
       </c>
       <c r="L9" s="1" t="inlineStr">
@@ -14452,12 +14466,12 @@
       </c>
       <c r="M9" s="1" t="inlineStr">
         <is>
-          <t>Borrower/true/17</t>
-        </is>
-      </c>
-      <c r="N9" s="1" t="inlineStr">
-        <is>
-          <t>2018-03-26</t>
+          <t>Borrower/true/6</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>2020-03-23</t>
         </is>
       </c>
       <c r="O9" s="1" t="inlineStr">
@@ -14470,11 +14484,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q9" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="Q9" s="33" t="inlineStr"/>
       <c r="R9" s="1" t="inlineStr">
         <is>
           <t>user</t>
@@ -14482,12 +14492,12 @@
       </c>
       <c r="S9" s="1" t="inlineStr">
         <is>
-          <t>WIDYUN3P</t>
+          <t>WUEGI81M</t>
         </is>
       </c>
       <c r="T9" s="1" t="inlineStr">
         <is>
-          <t>HSMGR01</t>
+          <t>SUPDEL01</t>
         </is>
       </c>
       <c r="U9" s="1" t="inlineStr">
@@ -14537,36 +14547,6 @@
           <t>Update</t>
         </is>
       </c>
-      <c r="H10" s="1" t="inlineStr">
-        <is>
-          <t>FACILITY-A_10102019150724YCL</t>
-        </is>
-      </c>
-      <c r="I10" s="1" t="inlineStr">
-        <is>
-          <t>TAM</t>
-        </is>
-      </c>
-      <c r="J10" s="1" t="inlineStr">
-        <is>
-          <t>3000062</t>
-        </is>
-      </c>
-      <c r="K10" s="1" t="inlineStr">
-        <is>
-          <t>CB001</t>
-        </is>
-      </c>
-      <c r="L10" s="1" t="inlineStr">
-        <is>
-          <t>AUSAG</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Borrower/false/5;Borrower/true/6|Borrower/false/5;Borrower/true/6</t>
-        </is>
-      </c>
       <c r="N10" s="1" t="inlineStr">
         <is>
           <t>2018-03-05</t>
@@ -14582,34 +14562,15 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q10" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="Q10" s="33" t="n"/>
       <c r="R10" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
       </c>
-      <c r="S10" s="1" t="inlineStr">
-        <is>
-          <t>O6DZ0NBQ</t>
-        </is>
-      </c>
-      <c r="T10" s="1" t="inlineStr">
-        <is>
-          <t>HSSUPR01</t>
-        </is>
-      </c>
       <c r="U10" s="1" t="inlineStr">
         <is>
           <t>Facility Change Transaction Released</t>
-        </is>
-      </c>
-      <c r="V10" s="1" t="inlineStr">
-        <is>
-          <t>ZONE3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GDE-6967 Updated variables on test suites Updated SAPWUL_CRE01 deal close date Updated correct data for UPD04 Updated correct effective date for SAPWUL_UPD06 Fixed kw to handle clicking the correct item on a table
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/SAPWUL/SAPWUL_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/SAPWUL/SAPWUL_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="565" firstSheet="1" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="32280" yWindow="870" windowWidth="21600" windowHeight="13995" tabRatio="565" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DealData" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -73,6 +73,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <color rgb="FF0070C0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -172,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -192,7 +198,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -214,6 +219,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,8 +532,8 @@
   </sheetPr>
   <dimension ref="A1:BT12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="BL1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BO2" sqref="BO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -596,8 +603,8 @@
     <col width="26.28515625" customWidth="1" style="1" min="66" max="66"/>
     <col width="34.85546875" customWidth="1" style="1" min="67" max="67"/>
     <col width="20" customWidth="1" style="1" min="68" max="68"/>
-    <col width="36.28515625" bestFit="1" customWidth="1" style="34" min="69" max="69"/>
-    <col width="12.85546875" bestFit="1" customWidth="1" style="34" min="70" max="70"/>
+    <col width="36.28515625" bestFit="1" customWidth="1" style="33" min="69" max="69"/>
+    <col width="12.85546875" bestFit="1" customWidth="1" style="33" min="70" max="70"/>
     <col width="18.85546875" customWidth="1" style="1" min="71" max="71"/>
     <col width="15.140625" customWidth="1" style="1" min="72" max="72"/>
   </cols>
@@ -987,12 +994,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SAPCRE01_14092020151257QHW</t>
+          <t>SAPCRE01_16092020114412TMY</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>D1_14092020151259VPE</t>
+          <t>D1_16092020114415YKV</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -1005,29 +1012,29 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I2" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J2" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K2" s="33" t="inlineStr">
+      <c r="I2" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J2" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K2" s="32" t="inlineStr">
         <is>
           <t>10-Mar-2020</t>
         </is>
       </c>
-      <c r="L2" s="33" t="inlineStr">
+      <c r="L2" s="32" t="inlineStr">
         <is>
           <t>23-Mar-2020</t>
         </is>
       </c>
-      <c r="M2" s="33" t="inlineStr">
-        <is>
-          <t>23-Mar-2020</t>
+      <c r="M2" s="37" t="inlineStr">
+        <is>
+          <t>20-Mar-2020</t>
         </is>
       </c>
       <c r="N2" s="1" t="inlineStr">
@@ -1301,12 +1308,12 @@
           <t>19-Dec-2011</t>
         </is>
       </c>
-      <c r="BQ2" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BR2" s="33" t="inlineStr">
+      <c r="BQ2" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BR2" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1373,17 +1380,17 @@
           <t>4</t>
         </is>
       </c>
-      <c r="K3" s="33" t="inlineStr">
+      <c r="K3" s="32" t="inlineStr">
         <is>
           <t>10-Mar-2020</t>
         </is>
       </c>
-      <c r="L3" s="33" t="inlineStr">
+      <c r="L3" s="32" t="inlineStr">
         <is>
           <t>23-Mar-2020</t>
         </is>
       </c>
-      <c r="M3" s="33" t="inlineStr">
+      <c r="M3" s="32" t="inlineStr">
         <is>
           <t>23-Mar-2020</t>
         </is>
@@ -1659,12 +1666,12 @@
           <t>19-Dec-2011</t>
         </is>
       </c>
-      <c r="BQ3" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BR3" s="33" t="inlineStr">
+      <c r="BQ3" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BR3" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1721,27 +1728,27 @@
           <t>5</t>
         </is>
       </c>
-      <c r="I4" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J4" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K4" s="33" t="inlineStr">
+      <c r="I4" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J4" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K4" s="32" t="inlineStr">
         <is>
           <t>10-Mar-2020</t>
         </is>
       </c>
-      <c r="L4" s="33" t="inlineStr">
+      <c r="L4" s="32" t="inlineStr">
         <is>
           <t>23-Mar-2020</t>
         </is>
       </c>
-      <c r="M4" s="33" t="inlineStr">
+      <c r="M4" s="32" t="inlineStr">
         <is>
           <t>23-Mar-2020</t>
         </is>
@@ -2017,12 +2024,12 @@
           <t>19-Dec-2011</t>
         </is>
       </c>
-      <c r="BQ4" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BR4" s="33" t="inlineStr">
+      <c r="BQ4" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BR4" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2375,12 +2382,12 @@
           <t>19-Dec-2011</t>
         </is>
       </c>
-      <c r="BQ5" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BR5" s="33" t="inlineStr">
+      <c r="BQ5" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BR5" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2733,12 +2740,12 @@
           <t>19-Dec-2011</t>
         </is>
       </c>
-      <c r="BQ6" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BR6" s="33" t="inlineStr">
+      <c r="BQ6" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BR6" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2755,7 +2762,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="33" t="inlineStr">
+      <c r="A7" s="32" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -2790,17 +2797,17 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="H7" s="33" t="inlineStr">
+      <c r="H7" s="32" t="inlineStr">
         <is>
           <t>27</t>
         </is>
       </c>
-      <c r="I7" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J7" s="33" t="inlineStr">
+      <c r="I7" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J7" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3091,12 +3098,12 @@
           <t>19-Dec-2011</t>
         </is>
       </c>
-      <c r="BQ7" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BR7" s="33" t="inlineStr">
+      <c r="BQ7" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BR7" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3113,7 +3120,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="33" t="inlineStr">
+      <c r="A8" s="32" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -3128,7 +3135,7 @@
           <t>SAPNEG09_</t>
         </is>
       </c>
-      <c r="D8" s="33" t="inlineStr">
+      <c r="D8" s="32" t="inlineStr">
         <is>
           <t>D7_</t>
         </is>
@@ -3148,17 +3155,17 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="H8" s="33" t="inlineStr">
+      <c r="H8" s="32" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="I8" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J8" s="33" t="inlineStr">
+      <c r="I8" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J8" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3449,12 +3456,12 @@
           <t>19-Dec-2011</t>
         </is>
       </c>
-      <c r="BQ8" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BR8" s="33" t="inlineStr">
+      <c r="BQ8" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BR8" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3471,7 +3478,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="33" t="inlineStr">
+      <c r="A9" s="32" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -3486,7 +3493,7 @@
           <t>SAPNEG10_</t>
         </is>
       </c>
-      <c r="D9" s="33" t="inlineStr">
+      <c r="D9" s="32" t="inlineStr">
         <is>
           <t>D8_</t>
         </is>
@@ -3506,17 +3513,17 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="H9" s="33" t="inlineStr">
+      <c r="H9" s="32" t="inlineStr">
         <is>
           <t>29</t>
         </is>
       </c>
-      <c r="I9" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J9" s="33" t="inlineStr">
+      <c r="I9" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J9" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3807,12 +3814,12 @@
           <t>19-Dec-2011</t>
         </is>
       </c>
-      <c r="BQ9" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BR9" s="33" t="inlineStr">
+      <c r="BQ9" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BR9" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3829,7 +3836,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="33" t="inlineStr">
+      <c r="A10" s="32" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -3844,7 +3851,7 @@
           <t>SAPUPD15_</t>
         </is>
       </c>
-      <c r="D10" s="33" t="inlineStr">
+      <c r="D10" s="32" t="inlineStr">
         <is>
           <t>D9_</t>
         </is>
@@ -3864,17 +3871,17 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="H10" s="33" t="inlineStr">
+      <c r="H10" s="32" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="I10" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J10" s="33" t="inlineStr">
+      <c r="I10" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J10" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -4165,12 +4172,12 @@
           <t>19-Dec-2011</t>
         </is>
       </c>
-      <c r="BQ10" s="29" t="inlineStr">
+      <c r="BQ10" s="28" t="inlineStr">
         <is>
           <t>LENDSHORT04137</t>
         </is>
       </c>
-      <c r="BR10" s="29" t="inlineStr">
+      <c r="BR10" s="28" t="inlineStr">
         <is>
           <t>Third Party</t>
         </is>
@@ -4180,19 +4187,19 @@
           <t>N</t>
         </is>
       </c>
-      <c r="BT10" s="31" t="inlineStr">
+      <c r="BT10" s="30" t="inlineStr">
         <is>
           <t>Lender Changed</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="33" t="inlineStr">
+      <c r="A11" s="32" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="B11" s="33" t="inlineStr">
+      <c r="B11" s="32" t="inlineStr">
         <is>
           <t>SAPWUL_UPD16</t>
         </is>
@@ -4202,7 +4209,7 @@
           <t>SAPUPD16_</t>
         </is>
       </c>
-      <c r="D11" s="33" t="inlineStr">
+      <c r="D11" s="32" t="inlineStr">
         <is>
           <t>D10</t>
         </is>
@@ -4222,17 +4229,17 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="H11" s="33" t="inlineStr">
+      <c r="H11" s="32" t="inlineStr">
         <is>
           <t>31</t>
         </is>
       </c>
-      <c r="I11" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J11" s="33" t="inlineStr">
+      <c r="I11" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J11" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -4462,12 +4469,12 @@
           <t>Start of next interest cycle</t>
         </is>
       </c>
-      <c r="BD11" s="29" t="inlineStr">
+      <c r="BD11" s="28" t="inlineStr">
         <is>
           <t>LENDSHORT04137</t>
         </is>
       </c>
-      <c r="BE11" s="33" t="inlineStr">
+      <c r="BE11" s="32" t="inlineStr">
         <is>
           <t>Melbourne, VIC,Australia</t>
         </is>
@@ -4493,12 +4500,12 @@
       <c r="BJ11" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="BK11" s="33" t="inlineStr">
+      <c r="BK11" s="32" t="inlineStr">
         <is>
           <t>Bloggs,  John</t>
         </is>
       </c>
-      <c r="BL11" s="33" t="inlineStr">
+      <c r="BL11" s="32" t="inlineStr">
         <is>
           <t>DDA</t>
         </is>
@@ -4528,7 +4535,7 @@
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="BR11" s="29" t="inlineStr">
+      <c r="BR11" s="28" t="inlineStr">
         <is>
           <t>Third Party</t>
         </is>
@@ -4538,14 +4545,14 @@
           <t>N</t>
         </is>
       </c>
-      <c r="BT11" s="31" t="inlineStr">
+      <c r="BT11" s="30" t="inlineStr">
         <is>
           <t>Lender Changed</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="33" t="inlineStr">
+      <c r="A12" s="32" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -4555,12 +4562,12 @@
           <t>SPAWUL_TERM01</t>
         </is>
       </c>
-      <c r="C12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D12" s="33" t="inlineStr">
+      <c r="C12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D12" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -4575,332 +4582,332 @@
           <t>S715012020161601VZG</t>
         </is>
       </c>
-      <c r="G12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H12" s="33" t="inlineStr">
+      <c r="G12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" s="32" t="inlineStr">
         <is>
           <t>32</t>
         </is>
       </c>
-      <c r="I12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="W12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Y12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AF12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AG12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AH12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AI12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AJ12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AK12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AL12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AM12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AN12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AO12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AP12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AQ12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AR12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AS12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AT12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AU12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AV12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AW12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AX12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AY12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AZ12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BA12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BB12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BC12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BD12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BE12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BF12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BG12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BH12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BI12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BJ12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BK12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BL12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BM12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BN12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BO12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BP12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BQ12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BR12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BS12" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="BT12" s="33" t="inlineStr">
+      <c r="I12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AM12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AN12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AO12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AR12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AS12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AT12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AU12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AV12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AW12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AX12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AY12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AZ12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BA12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BB12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BC12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BD12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BE12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BF12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BG12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BH12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BI12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BJ12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BK12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BL12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BM12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BN12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BO12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BP12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BQ12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BR12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BS12" s="32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="BT12" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -4922,9 +4929,9 @@
   <dimension ref="A1:BI33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AF1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="AE1" activePane="topRight" state="frozen"/>
       <selection activeCell="B8" sqref="B8"/>
-      <selection pane="topRight" activeCell="AK7" sqref="AK7"/>
+      <selection pane="topRight" activeCell="AF24" sqref="AF24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4963,7 +4970,7 @@
     <col width="34.85546875" customWidth="1" style="1" min="33" max="33"/>
     <col width="21" customWidth="1" style="1" min="34" max="34"/>
     <col width="23.42578125" customWidth="1" style="1" min="35" max="35"/>
-    <col width="33" customWidth="1" style="1" min="36" max="36"/>
+    <col width="50.42578125" customWidth="1" style="1" min="36" max="36"/>
     <col width="31.42578125" customWidth="1" style="1" min="37" max="37"/>
     <col width="31.85546875" customWidth="1" style="1" min="38" max="38"/>
     <col width="30.140625" customWidth="1" style="1" min="39" max="39"/>
@@ -4972,8 +4979,8 @@
     <col width="34.7109375" customWidth="1" style="1" min="42" max="42"/>
     <col width="21.5703125" bestFit="1" customWidth="1" style="1" min="43" max="43"/>
     <col width="28.28515625" bestFit="1" customWidth="1" style="1" min="44" max="44"/>
-    <col width="23.42578125" bestFit="1" customWidth="1" style="34" min="45" max="45"/>
-    <col width="19.7109375" customWidth="1" style="34" min="46" max="46"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" style="33" min="45" max="45"/>
+    <col width="19.7109375" customWidth="1" style="33" min="46" max="46"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.9" customFormat="1" customHeight="1" s="4" thickBot="1">
@@ -5241,15 +5248,15 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SAPCRE01_14092020151257QHW</t>
+          <t>SAPCRE01_16092020114412TMY</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FACILITY-A_14092020152142</t>
-        </is>
-      </c>
-      <c r="I2" s="33" t="inlineStr">
+          <t>FACILITY-A_16092020130140JBR</t>
+        </is>
+      </c>
+      <c r="I2" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -5274,22 +5281,22 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N2" s="33" t="inlineStr">
+      <c r="N2" s="32" t="inlineStr">
         <is>
           <t>10-Mar-2020</t>
         </is>
       </c>
-      <c r="O2" s="33" t="inlineStr">
+      <c r="O2" s="32" t="inlineStr">
         <is>
           <t>23-Mar-2020</t>
         </is>
       </c>
-      <c r="P2" s="33" t="inlineStr">
+      <c r="P2" s="32" t="inlineStr">
         <is>
           <t>17-Mar-2023</t>
         </is>
       </c>
-      <c r="Q2" s="33" t="inlineStr">
+      <c r="Q2" s="32" t="inlineStr">
         <is>
           <t>17-Mar-2023</t>
         </is>
@@ -5369,7 +5376,7 @@
           <t>0116 - AU / Stone Fruit Growing</t>
         </is>
       </c>
-      <c r="AG2" s="7" t="inlineStr">
+      <c r="AG2" s="16" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
@@ -5481,7 +5488,7 @@
           <t>FACILITY-B_10092020095510</t>
         </is>
       </c>
-      <c r="I3" s="33" t="inlineStr">
+      <c r="I3" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -5506,22 +5513,22 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N3" s="33" t="inlineStr">
+      <c r="N3" s="32" t="inlineStr">
         <is>
           <t>10-Mar-2020</t>
         </is>
       </c>
-      <c r="O3" s="33" t="inlineStr">
+      <c r="O3" s="32" t="inlineStr">
         <is>
           <t>23-Mar-2020</t>
         </is>
       </c>
-      <c r="P3" s="33" t="inlineStr">
+      <c r="P3" s="32" t="inlineStr">
         <is>
           <t>17-Mar-2023</t>
         </is>
       </c>
-      <c r="Q3" s="33" t="inlineStr">
+      <c r="Q3" s="32" t="inlineStr">
         <is>
           <t>17-Mar-2023</t>
         </is>
@@ -5713,7 +5720,7 @@
           <t>FACILITY-C_10092020100234</t>
         </is>
       </c>
-      <c r="I4" s="33" t="inlineStr">
+      <c r="I4" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -5738,22 +5745,22 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N4" s="33" t="inlineStr">
+      <c r="N4" s="32" t="inlineStr">
         <is>
           <t>10-Mar-2020</t>
         </is>
       </c>
-      <c r="O4" s="33" t="inlineStr">
+      <c r="O4" s="32" t="inlineStr">
         <is>
           <t>23-Mar-2020</t>
         </is>
       </c>
-      <c r="P4" s="33" t="inlineStr">
+      <c r="P4" s="32" t="inlineStr">
         <is>
           <t>17-Mar-2023</t>
         </is>
       </c>
-      <c r="Q4" s="33" t="inlineStr">
+      <c r="Q4" s="32" t="inlineStr">
         <is>
           <t>17-Mar-2023</t>
         </is>
@@ -5945,7 +5952,7 @@
           <t>FACILITY-D_10092020100955</t>
         </is>
       </c>
-      <c r="I5" s="33" t="inlineStr">
+      <c r="I5" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -5970,22 +5977,22 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N5" s="33" t="inlineStr">
+      <c r="N5" s="32" t="inlineStr">
         <is>
           <t>10-Mar-2020</t>
         </is>
       </c>
-      <c r="O5" s="33" t="inlineStr">
+      <c r="O5" s="32" t="inlineStr">
         <is>
           <t>23-Mar-2020</t>
         </is>
       </c>
-      <c r="P5" s="33" t="inlineStr">
+      <c r="P5" s="32" t="inlineStr">
         <is>
           <t>17-Mar-2023</t>
         </is>
       </c>
-      <c r="Q5" s="33" t="inlineStr">
+      <c r="Q5" s="32" t="inlineStr">
         <is>
           <t>17-Mar-2023</t>
         </is>
@@ -6177,7 +6184,7 @@
           <t>FACILITY-E_02032020175238</t>
         </is>
       </c>
-      <c r="I6" s="33" t="inlineStr">
+      <c r="I6" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -6202,22 +6209,22 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N6" s="33" t="inlineStr">
+      <c r="N6" s="32" t="inlineStr">
         <is>
           <t>10-Mar-2020</t>
         </is>
       </c>
-      <c r="O6" s="33" t="inlineStr">
+      <c r="O6" s="32" t="inlineStr">
         <is>
           <t>23-Mar-2020</t>
         </is>
       </c>
-      <c r="P6" s="33" t="inlineStr">
+      <c r="P6" s="32" t="inlineStr">
         <is>
           <t>17-Mar-2023</t>
         </is>
       </c>
-      <c r="Q6" s="33" t="inlineStr">
+      <c r="Q6" s="32" t="inlineStr">
         <is>
           <t>17-Mar-2023</t>
         </is>
@@ -6409,7 +6416,7 @@
           <t>FACILITY-F_04102019090040WIV</t>
         </is>
       </c>
-      <c r="I7" s="33" t="inlineStr">
+      <c r="I7" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -6641,7 +6648,7 @@
           <t>FACILITY-G_04102019090554EQE</t>
         </is>
       </c>
-      <c r="I8" s="33" t="inlineStr">
+      <c r="I8" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -6873,7 +6880,7 @@
           <t>FACILITY-H_04102019091110BRY</t>
         </is>
       </c>
-      <c r="I9" s="33" t="inlineStr">
+      <c r="I9" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -7090,22 +7097,22 @@
           <t>5</t>
         </is>
       </c>
-      <c r="F10" s="27" t="inlineStr">
+      <c r="F10" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>SAPCRE01_25112019135037EUE</t>
+          <t>SAPCRE01_16092020114412TMY</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>FACILITY-A_25112019135641JGG</t>
-        </is>
-      </c>
-      <c r="I10" s="33" t="inlineStr">
+          <t>FACILITY-A_16092020115532</t>
+        </is>
+      </c>
+      <c r="I10" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -7322,22 +7329,22 @@
           <t>6</t>
         </is>
       </c>
-      <c r="F11" s="27" t="inlineStr">
+      <c r="F11" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>SAPCRE01_09102019095641EBH</t>
+          <t>SAPCRE01_16092020114412TMY</t>
         </is>
       </c>
       <c r="H11" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_09102019102737HHJ</t>
-        </is>
-      </c>
-      <c r="I11" s="33" t="inlineStr">
+          <t>FACILITY-A_16092020130140JBR</t>
+        </is>
+      </c>
+      <c r="I11" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -7554,22 +7561,22 @@
           <t>7</t>
         </is>
       </c>
-      <c r="F12" s="27" t="inlineStr">
+      <c r="F12" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="G12" s="1" t="inlineStr">
         <is>
-          <t>SAPCRE01_09102019095641EBH</t>
+          <t>SAPCRE01_16092020114412TMY</t>
         </is>
       </c>
       <c r="H12" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_09102019102737HHJ</t>
-        </is>
-      </c>
-      <c r="I12" s="33" t="inlineStr">
+          <t>FACILITY-A_16092020130140JBR</t>
+        </is>
+      </c>
+      <c r="I12" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -7689,7 +7696,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AG12" s="16" t="inlineStr">
+      <c r="AG12" s="34" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - OBU</t>
         </is>
@@ -7786,22 +7793,22 @@
           <t>8</t>
         </is>
       </c>
-      <c r="F13" s="27" t="inlineStr">
+      <c r="F13" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="G13" s="1" t="inlineStr">
         <is>
-          <t>SAPCRE01_14092020151257QHW</t>
+          <t>SAPCRE01_16092020114412TMY</t>
         </is>
       </c>
       <c r="H13" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_14092020152142</t>
-        </is>
-      </c>
-      <c r="I13" s="33" t="inlineStr">
+          <t>FACILITY-A_16092020130140JBR</t>
+        </is>
+      </c>
+      <c r="I13" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -7811,9 +7818,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K13" s="36" t="inlineStr">
-        <is>
-          <t>Term</t>
+      <c r="K13" s="35" t="inlineStr">
+        <is>
+          <t>Revolver</t>
         </is>
       </c>
       <c r="L13" s="15" t="inlineStr">
@@ -7921,9 +7928,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AG13" s="35" t="inlineStr">
-        <is>
-          <t>Commonwealth Bank of Australia - DBU</t>
+      <c r="AG13" s="34" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - OBU</t>
         </is>
       </c>
       <c r="AH13" s="7" t="inlineStr">
@@ -8018,22 +8025,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="F14" s="27" t="inlineStr">
+      <c r="F14" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="G14" s="1" t="inlineStr">
         <is>
-          <t>SAPCRE01_10102019150426QEP</t>
+          <t>SAPCRE01_15092020115506GJL</t>
         </is>
       </c>
       <c r="H14" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_10102019150724YCL</t>
-        </is>
-      </c>
-      <c r="I14" s="33" t="inlineStr">
+          <t>FACILITY-A_15092020120742</t>
+        </is>
+      </c>
+      <c r="I14" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -8043,9 +8050,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K14" s="14" t="inlineStr">
-        <is>
-          <t>Term</t>
+      <c r="K14" s="35" t="inlineStr">
+        <is>
+          <t>Revolver</t>
         </is>
       </c>
       <c r="L14" s="15" t="inlineStr">
@@ -8265,22 +8272,22 @@
           <t>10</t>
         </is>
       </c>
-      <c r="F15" s="27" t="inlineStr">
+      <c r="F15" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="G15" s="1" t="inlineStr">
         <is>
-          <t>SAPCRE01_07102019090234GKV</t>
+          <t>SAPCRE01_16092020114412TMY</t>
         </is>
       </c>
       <c r="H15" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_07102019093752KLO</t>
-        </is>
-      </c>
-      <c r="I15" s="33" t="inlineStr">
+          <t>FACILITY-A_16092020130140JBR</t>
+        </is>
+      </c>
+      <c r="I15" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -8310,9 +8317,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O15" s="17" t="inlineStr">
-        <is>
-          <t>05-Mar-2018</t>
+      <c r="O15" s="36" t="inlineStr">
+        <is>
+          <t>22-Mar-2020</t>
         </is>
       </c>
       <c r="P15" s="15" t="inlineStr">
@@ -8400,7 +8407,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AG15" s="7" t="inlineStr">
+      <c r="AG15" s="35" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - OBU</t>
         </is>
@@ -8497,7 +8504,7 @@
           <t>11</t>
         </is>
       </c>
-      <c r="F16" s="27" t="inlineStr">
+      <c r="F16" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -8512,7 +8519,7 @@
           <t>FACILITY-A_11092020115319</t>
         </is>
       </c>
-      <c r="I16" s="33" t="inlineStr">
+      <c r="I16" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -8729,7 +8736,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="F17" s="27" t="inlineStr">
+      <c r="F17" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -8961,7 +8968,7 @@
           <t>13</t>
         </is>
       </c>
-      <c r="F18" s="27" t="inlineStr">
+      <c r="F18" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -8976,7 +8983,7 @@
           <t>FACILITY-A_10102019150724YCL</t>
         </is>
       </c>
-      <c r="I18" s="33" t="inlineStr">
+      <c r="I18" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -9193,7 +9200,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="F19" s="27" t="inlineStr">
+      <c r="F19" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -9208,7 +9215,7 @@
           <t>FACILITY-A_11122019145735</t>
         </is>
       </c>
-      <c r="I19" s="33" t="inlineStr">
+      <c r="I19" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -9425,7 +9432,7 @@
           <t>15</t>
         </is>
       </c>
-      <c r="F20" s="27" t="inlineStr">
+      <c r="F20" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -9440,7 +9447,7 @@
           <t>FACILITY-A_10102019150724YCL</t>
         </is>
       </c>
-      <c r="I20" s="33" t="inlineStr">
+      <c r="I20" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -9590,12 +9597,12 @@
           <t>Coll Deposit by Agent-DSRA</t>
         </is>
       </c>
-      <c r="AM20" s="18" t="inlineStr">
+      <c r="AM20" s="17" t="inlineStr">
         <is>
           <t>19-Dec-2018</t>
         </is>
       </c>
-      <c r="AN20" s="18" t="inlineStr">
+      <c r="AN20" s="17" t="inlineStr">
         <is>
           <t>19-Dec-2020</t>
         </is>
@@ -9651,7 +9658,7 @@
           <t>16</t>
         </is>
       </c>
-      <c r="F21" s="27" t="inlineStr">
+      <c r="F21" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -9666,7 +9673,7 @@
           <t>FACILITY-A_10102019150724YCL</t>
         </is>
       </c>
-      <c r="I21" s="33" t="inlineStr">
+      <c r="I21" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -9816,12 +9823,12 @@
           <t>Coll. Deposit at BLB- DSRA</t>
         </is>
       </c>
-      <c r="AM21" s="18" t="inlineStr">
+      <c r="AM21" s="17" t="inlineStr">
         <is>
           <t>19-Dec-2018</t>
         </is>
       </c>
-      <c r="AN21" s="18" t="inlineStr">
+      <c r="AN21" s="17" t="inlineStr">
         <is>
           <t>19-Jan-2022</t>
         </is>
@@ -9881,7 +9888,7 @@
           <t>17</t>
         </is>
       </c>
-      <c r="F22" s="27" t="inlineStr">
+      <c r="F22" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -9896,7 +9903,7 @@
           <t>FACILITY-A_11122019145735</t>
         </is>
       </c>
-      <c r="I22" s="33" t="inlineStr">
+      <c r="I22" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -10113,7 +10120,7 @@
           <t>18</t>
         </is>
       </c>
-      <c r="F23" s="27" t="inlineStr">
+      <c r="F23" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -10128,7 +10135,7 @@
           <t>FACILITY-A_10102019150724YCL</t>
         </is>
       </c>
-      <c r="I23" s="33" t="inlineStr">
+      <c r="I23" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -10278,12 +10285,12 @@
           <t>Coll. Deposit at BLB- DSRA</t>
         </is>
       </c>
-      <c r="AM23" s="18" t="inlineStr">
+      <c r="AM23" s="17" t="inlineStr">
         <is>
           <t>19-Dec-2018</t>
         </is>
       </c>
-      <c r="AN23" s="18" t="inlineStr">
+      <c r="AN23" s="17" t="inlineStr">
         <is>
           <t>19-Feb-2022</t>
         </is>
@@ -10358,7 +10365,7 @@
           <t>FACILITY-I_10122019192143</t>
         </is>
       </c>
-      <c r="I24" s="33" t="inlineStr">
+      <c r="I24" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -10383,12 +10390,12 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N24" s="33" t="inlineStr">
+      <c r="N24" s="32" t="inlineStr">
         <is>
           <t>28-Feb-2013</t>
         </is>
       </c>
-      <c r="O24" s="33" t="inlineStr">
+      <c r="O24" s="32" t="inlineStr">
         <is>
           <t>28-Feb-2013</t>
         </is>
@@ -10590,7 +10597,7 @@
           <t>FACILITY-E_04102019083946SEN</t>
         </is>
       </c>
-      <c r="I25" s="33" t="inlineStr">
+      <c r="I25" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -10615,7 +10622,7 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N25" s="33" t="inlineStr">
+      <c r="N25" s="32" t="inlineStr">
         <is>
           <t>28-Feb-2013</t>
         </is>
@@ -10822,7 +10829,7 @@
           <t>FACILITY-K_10122019193418</t>
         </is>
       </c>
-      <c r="I26" s="33" t="inlineStr">
+      <c r="I26" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -10847,7 +10854,7 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N26" s="33" t="inlineStr">
+      <c r="N26" s="32" t="inlineStr">
         <is>
           <t>28-Feb-2013</t>
         </is>
@@ -11029,7 +11036,7 @@
           <t>SAPNEG09_A_</t>
         </is>
       </c>
-      <c r="D27" s="33" t="inlineStr">
+      <c r="D27" s="32" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -11039,7 +11046,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F27" s="27" t="inlineStr">
+      <c r="F27" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -11054,7 +11061,7 @@
           <t>SAPNEG09_A_13122019115619</t>
         </is>
       </c>
-      <c r="I27" s="33" t="inlineStr">
+      <c r="I27" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -11079,12 +11086,12 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N27" s="33" t="inlineStr">
+      <c r="N27" s="32" t="inlineStr">
         <is>
           <t>05-Mar-2013</t>
         </is>
       </c>
-      <c r="O27" s="27" t="inlineStr">
+      <c r="O27" s="26" t="inlineStr">
         <is>
           <t>26-Mar-2013</t>
         </is>
@@ -11224,12 +11231,12 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AQ27" s="29" t="inlineStr">
+      <c r="AQ27" s="28" t="inlineStr">
         <is>
           <t>1000.00</t>
         </is>
       </c>
-      <c r="AR27" s="29" t="inlineStr">
+      <c r="AR27" s="28" t="inlineStr">
         <is>
           <t>10.0000%</t>
         </is>
@@ -11246,7 +11253,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="33" t="inlineStr">
+      <c r="A28" s="32" t="inlineStr">
         <is>
           <t>27</t>
         </is>
@@ -11261,7 +11268,7 @@
           <t>FACILITY-L_</t>
         </is>
       </c>
-      <c r="D28" s="33" t="inlineStr">
+      <c r="D28" s="32" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -11271,7 +11278,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F28" s="27" t="inlineStr">
+      <c r="F28" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -11286,7 +11293,7 @@
           <t>FACILITY-L_10122019162854CXW</t>
         </is>
       </c>
-      <c r="I28" s="33" t="inlineStr">
+      <c r="I28" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -11311,7 +11318,7 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N28" s="33" t="inlineStr">
+      <c r="N28" s="32" t="inlineStr">
         <is>
           <t>28-Feb-2013</t>
         </is>
@@ -11478,7 +11485,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="33" t="inlineStr">
+      <c r="A29" s="32" t="inlineStr">
         <is>
           <t>28</t>
         </is>
@@ -11493,17 +11500,17 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D29" s="27" t="inlineStr">
+      <c r="D29" s="26" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E29" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F29" s="27" t="inlineStr">
+      <c r="E29" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -11518,7 +11525,7 @@
           <t>FACILITY-A_11122019145735</t>
         </is>
       </c>
-      <c r="I29" s="33" t="inlineStr">
+      <c r="I29" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -11598,7 +11605,7 @@
           <t>JOBERN</t>
         </is>
       </c>
-      <c r="Y29" s="28" t="inlineStr">
+      <c r="Y29" s="27" t="inlineStr">
         <is>
           <t>TONY</t>
         </is>
@@ -11710,7 +11717,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="33" t="inlineStr">
+      <c r="A30" s="32" t="inlineStr">
         <is>
           <t>29</t>
         </is>
@@ -11725,7 +11732,7 @@
           <t>SAPNEG10_</t>
         </is>
       </c>
-      <c r="D30" s="33" t="inlineStr">
+      <c r="D30" s="32" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -11735,7 +11742,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F30" s="27" t="inlineStr">
+      <c r="F30" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -11750,7 +11757,7 @@
           <t>SAPNEG1009012020181905</t>
         </is>
       </c>
-      <c r="I30" s="33" t="inlineStr">
+      <c r="I30" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -11775,12 +11782,12 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N30" s="33" t="inlineStr">
+      <c r="N30" s="32" t="inlineStr">
         <is>
           <t>05-Mar-2013</t>
         </is>
       </c>
-      <c r="O30" s="27" t="inlineStr">
+      <c r="O30" s="26" t="inlineStr">
         <is>
           <t>26-Mar-2013</t>
         </is>
@@ -11900,12 +11907,12 @@
           <t>Coll Deposit by Agent-DSRA</t>
         </is>
       </c>
-      <c r="AM30" s="18" t="inlineStr">
+      <c r="AM30" s="17" t="inlineStr">
         <is>
           <t>19-Dec-2018</t>
         </is>
       </c>
-      <c r="AN30" s="30" t="inlineStr">
+      <c r="AN30" s="29" t="inlineStr">
         <is>
           <t>18-Dec-2020</t>
         </is>
@@ -11940,7 +11947,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="33" t="inlineStr">
+      <c r="A31" s="32" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -11955,7 +11962,7 @@
           <t>SAPUPD15_</t>
         </is>
       </c>
-      <c r="D31" s="33" t="inlineStr">
+      <c r="D31" s="32" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -11965,7 +11972,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F31" s="27" t="inlineStr">
+      <c r="F31" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -11980,7 +11987,7 @@
           <t>SAPUPD15_13012020182425</t>
         </is>
       </c>
-      <c r="I31" s="33" t="inlineStr">
+      <c r="I31" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -12005,12 +12012,12 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N31" s="33" t="inlineStr">
+      <c r="N31" s="32" t="inlineStr">
         <is>
           <t>05-Mar-2013</t>
         </is>
       </c>
-      <c r="O31" s="27" t="inlineStr">
+      <c r="O31" s="26" t="inlineStr">
         <is>
           <t>26-Mar-2013</t>
         </is>
@@ -12172,7 +12179,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="33" t="inlineStr">
+      <c r="A32" s="32" t="inlineStr">
         <is>
           <t>31</t>
         </is>
@@ -12187,7 +12194,7 @@
           <t>SAPUPD16_</t>
         </is>
       </c>
-      <c r="D32" s="33" t="inlineStr">
+      <c r="D32" s="32" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -12197,7 +12204,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F32" s="27" t="inlineStr">
+      <c r="F32" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -12212,7 +12219,7 @@
           <t>SAPUPD16_14012020140701</t>
         </is>
       </c>
-      <c r="I32" s="33" t="inlineStr">
+      <c r="I32" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -12237,12 +12244,12 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="N32" s="33" t="inlineStr">
+      <c r="N32" s="32" t="inlineStr">
         <is>
           <t>05-Mar-2013</t>
         </is>
       </c>
-      <c r="O32" s="27" t="inlineStr">
+      <c r="O32" s="26" t="inlineStr">
         <is>
           <t>26-Mar-2013</t>
         </is>
@@ -12404,7 +12411,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="33" t="inlineStr">
+      <c r="A33" s="32" t="inlineStr">
         <is>
           <t>32</t>
         </is>
@@ -12419,17 +12426,17 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D33" s="33" t="inlineStr">
+      <c r="D33" s="32" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E33" s="33" t="inlineStr">
+      <c r="E33" s="32" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="F33" s="27" t="inlineStr">
+      <c r="F33" s="26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -12444,137 +12451,137 @@
           <t>S115012020162212OHT</t>
         </is>
       </c>
-      <c r="I33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K33" s="27" t="inlineStr">
+      <c r="I33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K33" s="26" t="inlineStr">
         <is>
           <t>Term</t>
         </is>
       </c>
-      <c r="L33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O33" s="27" t="inlineStr">
+      <c r="L33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O33" s="26" t="inlineStr">
         <is>
           <t>26-Jul-2018</t>
         </is>
       </c>
-      <c r="P33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="W33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X33" s="27" t="inlineStr">
+      <c r="P33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X33" s="26" t="inlineStr">
         <is>
           <t>ESPS51715027</t>
         </is>
       </c>
-      <c r="Y33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AF33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AG33" s="27" t="inlineStr">
+      <c r="Y33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG33" s="26" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
-      <c r="AH33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AI33" s="27" t="inlineStr">
+      <c r="AH33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI33" s="26" t="inlineStr">
         <is>
           <t>Agency Australia</t>
         </is>
@@ -12584,47 +12591,47 @@
           <t>Facility Change Transaction Released</t>
         </is>
       </c>
-      <c r="AK33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AL33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AM33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AN33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AO33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AP33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AQ33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AR33" s="27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AS33" s="27" t="inlineStr">
+      <c r="AK33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AM33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AN33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AO33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AR33" s="26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AS33" s="26" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -12662,61 +12669,61 @@
     <col width="22.42578125" customWidth="1" style="1" min="9" max="9"/>
     <col width="15.5703125" customWidth="1" style="1" min="10" max="10"/>
     <col width="14.5703125" customWidth="1" style="1" min="11" max="11"/>
-    <col width="22.140625" bestFit="1" customWidth="1" style="34" min="12" max="12"/>
+    <col width="22.140625" bestFit="1" customWidth="1" style="33" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customFormat="1" customHeight="1" s="19" thickBot="1">
-      <c r="A1" s="20" t="inlineStr">
+    <row r="1" ht="13.5" customFormat="1" customHeight="1" s="18" thickBot="1">
+      <c r="A1" s="19" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="20" t="inlineStr">
+      <c r="B1" s="19" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="21" t="inlineStr">
+      <c r="C1" s="20" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="D1" s="19" t="inlineStr">
+      <c r="D1" s="18" t="inlineStr">
         <is>
           <t>Interest_AddItem</t>
         </is>
       </c>
-      <c r="E1" s="19" t="inlineStr">
+      <c r="E1" s="18" t="inlineStr">
         <is>
           <t>Interest_OptionName</t>
         </is>
       </c>
-      <c r="F1" s="19" t="inlineStr">
+      <c r="F1" s="18" t="inlineStr">
         <is>
           <t>Interest_RateBasis</t>
         </is>
       </c>
-      <c r="G1" s="19" t="inlineStr">
+      <c r="G1" s="18" t="inlineStr">
         <is>
           <t>Interest_SpreadValue</t>
         </is>
       </c>
-      <c r="H1" s="19" t="inlineStr">
+      <c r="H1" s="18" t="inlineStr">
         <is>
           <t>Interest_BaseRateCode_Formula</t>
         </is>
       </c>
-      <c r="I1" s="19" t="inlineStr">
+      <c r="I1" s="18" t="inlineStr">
         <is>
           <t>Interest_BaseRateCode</t>
         </is>
       </c>
-      <c r="J1" s="19" t="inlineStr">
+      <c r="J1" s="18" t="inlineStr">
         <is>
           <t>Penalty_Spread</t>
         </is>
       </c>
-      <c r="K1" s="19" t="inlineStr">
+      <c r="K1" s="18" t="inlineStr">
         <is>
           <t>Penalty_Status</t>
         </is>
@@ -12740,7 +12747,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_14092020152142</t>
+          <t>FACILITY-A_16092020115532</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -12763,17 +12770,17 @@
           <t>1.7</t>
         </is>
       </c>
-      <c r="H2" s="22" t="inlineStr">
+      <c r="H2" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="I2" s="22" t="inlineStr">
+      <c r="I2" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="J2" s="23" t="inlineStr">
+      <c r="J2" s="22" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -12825,17 +12832,17 @@
           <t>1.7</t>
         </is>
       </c>
-      <c r="H3" s="22" t="inlineStr">
+      <c r="H3" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="I3" s="22" t="inlineStr">
+      <c r="I3" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="J3" s="23" t="inlineStr">
+      <c r="J3" s="22" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -12887,17 +12894,17 @@
           <t>1.7</t>
         </is>
       </c>
-      <c r="H4" s="22" t="inlineStr">
+      <c r="H4" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="I4" s="22" t="inlineStr">
+      <c r="I4" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="J4" s="23" t="inlineStr">
+      <c r="J4" s="22" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -12949,17 +12956,17 @@
           <t>1.7</t>
         </is>
       </c>
-      <c r="H5" s="22" t="inlineStr">
+      <c r="H5" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="I5" s="22" t="inlineStr">
+      <c r="I5" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="J5" s="23" t="inlineStr">
+      <c r="J5" s="22" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -13011,17 +13018,17 @@
           <t>1.7</t>
         </is>
       </c>
-      <c r="H6" s="22" t="inlineStr">
+      <c r="H6" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="I6" s="22" t="inlineStr">
+      <c r="I6" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="J6" s="23" t="inlineStr">
+      <c r="J6" s="22" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -13073,17 +13080,17 @@
           <t>1.7</t>
         </is>
       </c>
-      <c r="H7" s="22" t="inlineStr">
+      <c r="H7" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="I7" s="22" t="inlineStr">
+      <c r="I7" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="J7" s="23" t="inlineStr">
+      <c r="J7" s="22" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -13135,17 +13142,17 @@
           <t>1.7</t>
         </is>
       </c>
-      <c r="H8" s="22" t="inlineStr">
+      <c r="H8" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="I8" s="22" t="inlineStr">
+      <c r="I8" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="J8" s="23" t="inlineStr">
+      <c r="J8" s="22" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -13197,17 +13204,17 @@
           <t>1.7</t>
         </is>
       </c>
-      <c r="H9" s="22" t="inlineStr">
+      <c r="H9" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="I9" s="22" t="inlineStr">
+      <c r="I9" s="21" t="inlineStr">
         <is>
           <t>FIX</t>
         </is>
       </c>
-      <c r="J9" s="23" t="inlineStr">
+      <c r="J9" s="22" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -13410,7 +13417,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="33" t="inlineStr">
+      <c r="A13" s="32" t="inlineStr">
         <is>
           <t>12</t>
         </is>
@@ -13472,7 +13479,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="33" t="inlineStr">
+      <c r="A14" s="32" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -13527,14 +13534,14 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="L14" s="33" t="inlineStr">
+      <c r="L14" s="32" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="33" t="inlineStr">
+      <c r="A15" s="32" t="inlineStr">
         <is>
           <t>14</t>
         </is>
@@ -13589,14 +13596,14 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="L15" s="33" t="inlineStr">
+      <c r="L15" s="32" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="33" t="inlineStr">
+      <c r="A16" s="32" t="inlineStr">
         <is>
           <t>15</t>
         </is>
@@ -13651,14 +13658,14 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="L16" s="33" t="inlineStr">
+      <c r="L16" s="32" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="33" t="inlineStr">
+      <c r="A17" s="32" t="inlineStr">
         <is>
           <t>16</t>
         </is>
@@ -13713,7 +13720,7 @@
           <t>Off</t>
         </is>
       </c>
-      <c r="L17" s="33" t="inlineStr">
+      <c r="L17" s="32" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -13735,8 +13742,8 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N12" sqref="N12"/>
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -13765,8 +13772,8 @@
     <col width="20.140625" customWidth="1" style="1" min="22" max="22"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.9" customHeight="1" s="34" thickBot="1">
-      <c r="A1" s="20" t="inlineStr">
+    <row r="1" ht="13.9" customHeight="1" s="33" thickBot="1">
+      <c r="A1" s="19" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
@@ -13781,17 +13788,17 @@
           <t>OtherPayloadVal_Clear</t>
         </is>
       </c>
-      <c r="D1" s="24" t="inlineStr">
+      <c r="D1" s="23" t="inlineStr">
         <is>
           <t>Payload_keys</t>
         </is>
       </c>
-      <c r="E1" s="24" t="inlineStr">
+      <c r="E1" s="23" t="inlineStr">
         <is>
           <t>customerExternalID_keys</t>
         </is>
       </c>
-      <c r="F1" s="24" t="inlineStr">
+      <c r="F1" s="23" t="inlineStr">
         <is>
           <t>internal_keys</t>
         </is>
@@ -13801,7 +13808,7 @@
           <t>Payload_action</t>
         </is>
       </c>
-      <c r="H1" s="25" t="inlineStr">
+      <c r="H1" s="24" t="inlineStr">
         <is>
           <t>Payload_facilityName</t>
         </is>
@@ -13826,7 +13833,7 @@
           <t>Payload_processingAreaCode</t>
         </is>
       </c>
-      <c r="M1" s="25" t="inlineStr">
+      <c r="M1" s="24" t="inlineStr">
         <is>
           <t>Payload_customerExternalID</t>
         </is>
@@ -13841,7 +13848,7 @@
           <t>Payload_status</t>
         </is>
       </c>
-      <c r="P1" s="26" t="inlineStr">
+      <c r="P1" s="25" t="inlineStr">
         <is>
           <t>Payload_hasExposure</t>
         </is>
@@ -13893,7 +13900,7 @@
           <t>Payload_effectiveDate</t>
         </is>
       </c>
-      <c r="D2" s="31" t="inlineStr">
+      <c r="D2" s="30" t="inlineStr">
         <is>
           <t>action|facilityName|facilityTypeCode|facilityControlNumber|owningBranchCode|processingAreaCode|effectiveDate|status|hasExposure</t>
         </is>
@@ -13915,7 +13922,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FACILITY-A_14092020152142</t>
+          <t>FACILITY-A_16092020115532</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -13925,7 +13932,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3000663</t>
+          <t>3000684</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -13958,7 +13965,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q2" s="33" t="n"/>
+      <c r="Q2" s="32" t="n"/>
       <c r="R2" s="1" t="inlineStr">
         <is>
           <t>user</t>
@@ -13966,7 +13973,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>WUEGI81M</t>
+          <t>-$EGLNUO</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
@@ -14066,7 +14073,7 @@
           <t>true|true|true</t>
         </is>
       </c>
-      <c r="Q3" s="33" t="n"/>
+      <c r="Q3" s="32" t="n"/>
       <c r="R3" s="1" t="inlineStr">
         <is>
           <t>user|user|user</t>
@@ -14125,9 +14132,9 @@
         </is>
       </c>
       <c r="G4" s="7" t="n"/>
-      <c r="Q4" s="33" t="n"/>
+      <c r="Q4" s="32" t="n"/>
     </row>
-    <row r="5" ht="13.5" customHeight="1" s="34">
+    <row r="5" ht="13.5" customHeight="1" s="33">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>4</t>
@@ -14164,9 +14171,9 @@
           <t>2018-03-26</t>
         </is>
       </c>
-      <c r="Q5" s="33" t="n"/>
+      <c r="Q5" s="32" t="n"/>
     </row>
-    <row r="6" ht="13.5" customHeight="1" s="34">
+    <row r="6" ht="13.5" customHeight="1" s="33">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>5</t>
@@ -14204,7 +14211,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>FACILITY-A_25112019135641JGG</t>
+          <t>FACILITY-A_16092020115532</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -14214,7 +14221,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>3000089</t>
+          <t>3000684</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -14229,14 +14236,10 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Borrower/true/5</t>
-        </is>
-      </c>
-      <c r="N6" s="33" t="inlineStr">
-        <is>
-          <t>2018-03-05</t>
-        </is>
-      </c>
+          <t>Borrower/true/6</t>
+        </is>
+      </c>
+      <c r="N6" s="32" t="n"/>
       <c r="O6" s="1" t="inlineStr">
         <is>
           <t>Active</t>
@@ -14247,11 +14250,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q6" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="Q6" s="32" t="n"/>
       <c r="R6" s="1" t="inlineStr">
         <is>
           <t>user</t>
@@ -14259,12 +14258,12 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>3AE1DQDF</t>
+          <t>-$EGLNUO</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>mmansuet</t>
+          <t>SUPDEL01</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -14278,7 +14277,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="13.5" customHeight="1" s="34">
+    <row r="7" ht="13.5" customHeight="1" s="33">
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>6</t>
@@ -14314,6 +14313,36 @@
           <t>Update</t>
         </is>
       </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>FACILITY-A_16092020130140JBR</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>RST</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>3000684</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>CB001</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>AUSAG</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Borrower/true/6</t>
+        </is>
+      </c>
       <c r="O7" s="1" t="inlineStr">
         <is>
           <t>Active</t>
@@ -14324,15 +14353,30 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q7" s="33" t="n"/>
+      <c r="Q7" s="32" t="n"/>
       <c r="R7" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
       </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>-$EGLNUO</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>INPDEL01</t>
+        </is>
+      </c>
       <c r="U7" s="1" t="inlineStr">
         <is>
           <t>Facility Rename</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>ZONE3</t>
         </is>
       </c>
     </row>
@@ -14372,9 +14416,39 @@
           <t>Update</t>
         </is>
       </c>
-      <c r="N8" s="1" t="inlineStr">
-        <is>
-          <t>2018-03-26</t>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>FACILITY-A_16092020130140JBR</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>RST</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>3000684</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>CB022</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>AUSAG</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Borrower/true/6</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>2020-03-23</t>
         </is>
       </c>
       <c r="O8" s="1" t="inlineStr">
@@ -14387,19 +14461,30 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q8" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="Q8" s="32" t="n"/>
       <c r="R8" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
       </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>-$EGLNUO</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>SUPDEL01</t>
+        </is>
+      </c>
       <c r="U8" s="1" t="inlineStr">
         <is>
           <t>Facility Change Transaction Released</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>ZONE3</t>
         </is>
       </c>
     </row>
@@ -14439,32 +14524,32 @@
           <t>Update</t>
         </is>
       </c>
-      <c r="H9" s="1" t="inlineStr">
-        <is>
-          <t>FACILITY-A_14092020152142</t>
-        </is>
-      </c>
-      <c r="I9" s="1" t="inlineStr">
-        <is>
-          <t>TAM</t>
-        </is>
-      </c>
-      <c r="J9" s="1" t="inlineStr">
-        <is>
-          <t>3000663</t>
-        </is>
-      </c>
-      <c r="K9" s="1" t="inlineStr">
-        <is>
-          <t>CB001</t>
-        </is>
-      </c>
-      <c r="L9" s="1" t="inlineStr">
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>FACILITY-A_16092020130140JBR</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>RST</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>3000684</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>CB022</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
         <is>
           <t>AUSNA</t>
         </is>
       </c>
-      <c r="M9" s="1" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>Borrower/true/6</t>
         </is>
@@ -14484,18 +14569,18 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q9" s="33" t="inlineStr"/>
+      <c r="Q9" s="32" t="n"/>
       <c r="R9" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
       </c>
-      <c r="S9" s="1" t="inlineStr">
-        <is>
-          <t>WUEGI81M</t>
-        </is>
-      </c>
-      <c r="T9" s="1" t="inlineStr">
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>-$EGLNUO</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
         <is>
           <t>SUPDEL01</t>
         </is>
@@ -14505,7 +14590,7 @@
           <t>Facility Change Transaction Released</t>
         </is>
       </c>
-      <c r="V9" s="1" t="inlineStr">
+      <c r="V9" t="inlineStr">
         <is>
           <t>ZONE3</t>
         </is>
@@ -14562,7 +14647,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q10" s="33" t="n"/>
+      <c r="Q10" s="32" t="n"/>
       <c r="R10" s="1" t="inlineStr">
         <is>
           <t>user</t>
@@ -14610,39 +14695,39 @@
           <t>Update</t>
         </is>
       </c>
-      <c r="H11" s="1" t="inlineStr">
-        <is>
-          <t>FACILITY-A_07102019093752KLO</t>
-        </is>
-      </c>
-      <c r="I11" s="1" t="inlineStr">
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>FACILITY-A_16092020130140JBR</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>RST</t>
         </is>
       </c>
-      <c r="J11" s="1" t="inlineStr">
-        <is>
-          <t>03000160</t>
-        </is>
-      </c>
-      <c r="K11" s="1" t="inlineStr">
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>3000684</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>CB022</t>
         </is>
       </c>
-      <c r="L11" s="1" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>AUSNA</t>
         </is>
       </c>
-      <c r="M11" s="1" t="inlineStr">
-        <is>
-          <t>Borrower/true/17</t>
-        </is>
-      </c>
-      <c r="N11" s="1" t="inlineStr">
-        <is>
-          <t>2018-03-05</t>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Borrower/true/6</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>2020-03-22</t>
         </is>
       </c>
       <c r="O11" s="1" t="inlineStr">
@@ -14655,24 +14740,20 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q11" s="33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="Q11" s="32" t="inlineStr"/>
       <c r="R11" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
       </c>
-      <c r="S11" s="1" t="inlineStr">
-        <is>
-          <t>WIDYUN3P</t>
-        </is>
-      </c>
-      <c r="T11" s="1" t="inlineStr">
-        <is>
-          <t>HSMGR01</t>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>-$EGLNUO</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>SUPDEL01</t>
         </is>
       </c>
       <c r="U11" s="1" t="inlineStr">
@@ -14680,7 +14761,7 @@
           <t>Facility Change Transaction Released</t>
         </is>
       </c>
-      <c r="V11" s="1" t="inlineStr">
+      <c r="V11" t="inlineStr">
         <is>
           <t>ZONE3</t>
         </is>
@@ -14767,7 +14848,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q12" s="33" t="inlineStr">
+      <c r="Q12" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -14874,7 +14955,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q13" s="33" t="inlineStr">
+      <c r="Q13" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -14986,7 +15067,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q14" s="33" t="inlineStr">
+      <c r="Q14" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -15098,7 +15179,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q15" s="33" t="inlineStr">
+      <c r="Q15" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -15180,7 +15261,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q16" s="33" t="inlineStr">
+      <c r="Q16" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -15277,7 +15358,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q17" s="33" t="inlineStr">
+      <c r="Q17" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -15359,7 +15440,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q18" s="33" t="inlineStr">
+      <c r="Q18" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -15456,7 +15537,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q19" s="33" t="inlineStr">
+      <c r="Q19" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -15488,7 +15569,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="33" t="inlineStr">
+      <c r="A20" s="32" t="inlineStr">
         <is>
           <t>19</t>
         </is>
@@ -15568,7 +15649,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q20" s="33" t="inlineStr">
+      <c r="Q20" s="32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -15600,7 +15681,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="33" t="inlineStr">
+      <c r="A21" s="32" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -15615,7 +15696,7 @@
           <t>Payload_effectiveDate</t>
         </is>
       </c>
-      <c r="D21" s="31" t="inlineStr">
+      <c r="D21" s="30" t="inlineStr">
         <is>
           <t>action|facilityName|facilityTypeCode|facilityControlNumber|owningBranchCode|processingAreaCode|effectiveDate|status|hasExposure|terminationDate</t>
         </is>
@@ -15630,7 +15711,7 @@
           <t>userType|facilityId|userId|eventDescription|zone</t>
         </is>
       </c>
-      <c r="G21" s="32" t="inlineStr">
+      <c r="G21" s="31" t="inlineStr">
         <is>
           <t>Terminated</t>
         </is>
@@ -15675,12 +15756,12 @@
           <t>Terminated</t>
         </is>
       </c>
-      <c r="P21" s="33" t="inlineStr">
+      <c r="P21" s="32" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="Q21" s="33" t="inlineStr">
+      <c r="Q21" s="32" t="inlineStr">
         <is>
           <t>2018-07-31</t>
         </is>
@@ -15732,11 +15813,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="29.85546875" bestFit="1" customWidth="1" style="34" min="1" max="1"/>
+    <col width="29.85546875" bestFit="1" customWidth="1" style="33" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="2" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
-      <c r="A2" s="25" t="inlineStr">
+    <row r="2" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
+      <c r="A2" s="24" t="inlineStr">
         <is>
           <t>Payload_facilityName</t>
         </is>
@@ -15747,7 +15828,7 @@
         </is>
       </c>
     </row>
-    <row r="3" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="3" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A3" s="10" t="inlineStr">
         <is>
           <t>Payload_facilityTypeCode</t>
@@ -15759,7 +15840,7 @@
         </is>
       </c>
     </row>
-    <row r="4" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="4" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A4" s="10" t="inlineStr">
         <is>
           <t>Payload_facilityControlNumber</t>
@@ -15771,7 +15852,7 @@
         </is>
       </c>
     </row>
-    <row r="5" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="5" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A5" s="10" t="inlineStr">
         <is>
           <t>Payload_owningBranchCode</t>
@@ -15783,7 +15864,7 @@
         </is>
       </c>
     </row>
-    <row r="6" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="6" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A6" s="10" t="inlineStr">
         <is>
           <t>Payload_processingAreaCode</t>
@@ -15795,8 +15876,8 @@
         </is>
       </c>
     </row>
-    <row r="7" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
-      <c r="A7" s="25" t="inlineStr">
+    <row r="7" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
+      <c r="A7" s="24" t="inlineStr">
         <is>
           <t>Payload_customerExternalID</t>
         </is>
@@ -15807,7 +15888,7 @@
         </is>
       </c>
     </row>
-    <row r="8" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="8" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Payload_effectiveDate</t>
@@ -15819,7 +15900,7 @@
         </is>
       </c>
     </row>
-    <row r="9" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="9" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Payload_status</t>
@@ -15831,8 +15912,8 @@
         </is>
       </c>
     </row>
-    <row r="10" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
-      <c r="A10" s="26" t="inlineStr">
+    <row r="10" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
+      <c r="A10" s="25" t="inlineStr">
         <is>
           <t>Payload_hasExposure</t>
         </is>
@@ -15843,7 +15924,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="11" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Payload_terminationDate</t>
@@ -15855,7 +15936,7 @@
         </is>
       </c>
     </row>
-    <row r="12" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="12" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Internal_userType</t>
@@ -15867,7 +15948,7 @@
         </is>
       </c>
     </row>
-    <row r="13" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="13" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A13" s="10" t="inlineStr">
         <is>
           <t>Internal_facilityId</t>
@@ -15879,7 +15960,7 @@
         </is>
       </c>
     </row>
-    <row r="14" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="14" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A14" s="10" t="inlineStr">
         <is>
           <t>Internal_userId</t>
@@ -15891,7 +15972,7 @@
         </is>
       </c>
     </row>
-    <row r="15" hidden="1" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="15" hidden="1" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A15" s="4" t="inlineStr">
         <is>
           <t>Internal_eventDescription</t>
@@ -15903,7 +15984,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="13.5" customHeight="1" s="34" thickBot="1">
+    <row r="16" ht="13.5" customHeight="1" s="33" thickBot="1">
       <c r="A16" s="10" t="inlineStr">
         <is>
           <t>Internal_zone</t>

</xml_diff>

<commit_message>
GDE-6969 fixes for SAPWUL_UPD08
Updated variables on test suite
Added Sapwul_hasTrigger column on FacilityData sheet
Fixed Enter key with correct value
Fixed argument issue Create Customer External ID List and Set SAPWUL
Test Data
Added step to convert payload_effectiveDate to correct format
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/SAPWUL/SAPWUL_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/SAPWUL/SAPWUL_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="32280" yWindow="870" windowWidth="21600" windowHeight="13995" tabRatio="565" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="565" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DealData" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,8 +21,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="10">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="11">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -80,6 +82,11 @@
       <family val="2"/>
       <color rgb="FFFF0000"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="8"/>
     </font>
   </fonts>
   <fills count="6">
@@ -178,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -221,6 +228,12 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="15" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,8 +545,8 @@
   </sheetPr>
   <dimension ref="A1:BT12"/>
   <sheetViews>
-    <sheetView topLeftCell="BL1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BO2" sqref="BO2"/>
+    <sheetView topLeftCell="BN1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BS1" sqref="BS1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -994,12 +1007,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SAPCRE01_16092020114412TMY</t>
+          <t>SAPCRE01_17092020120338XPU</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>D1_16092020114415YKV</t>
+          <t>D1_17092020120341RAL</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -4928,10 +4941,10 @@
   </sheetPr>
   <dimension ref="A1:BI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AE1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AT1" activePane="topRight" state="frozen"/>
       <selection activeCell="B8" sqref="B8"/>
-      <selection pane="topRight" activeCell="AF24" sqref="AF24"/>
+      <selection pane="topRight" activeCell="AU1" sqref="AU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4981,6 +4994,7 @@
     <col width="28.28515625" bestFit="1" customWidth="1" style="1" min="44" max="44"/>
     <col width="23.42578125" bestFit="1" customWidth="1" style="33" min="45" max="45"/>
     <col width="19.7109375" customWidth="1" style="33" min="46" max="46"/>
+    <col width="18.85546875" bestFit="1" customWidth="1" style="33" min="47" max="47"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.9" customFormat="1" customHeight="1" s="4" thickBot="1">
@@ -5214,6 +5228,11 @@
           <t>Primary_Headers</t>
         </is>
       </c>
+      <c r="AU1" s="4" t="inlineStr">
+        <is>
+          <t>Sapwul_hasTrigger</t>
+        </is>
+      </c>
     </row>
     <row r="2" customFormat="1" s="7">
       <c r="A2" s="7" t="inlineStr">
@@ -5248,12 +5267,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SAPCRE01_16092020114412TMY</t>
+          <t>SAPCRE01_17092020120338XPU</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FACILITY-A_16092020130140JBR</t>
+          <t>FACILITY-A_17092020121428</t>
         </is>
       </c>
       <c r="I2" s="32" t="inlineStr">
@@ -5442,6 +5461,11 @@
         </is>
       </c>
       <c r="AT2" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AU2" s="5" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -5678,6 +5702,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="4" customFormat="1" s="7">
       <c r="A4" s="7" t="inlineStr">
@@ -5910,6 +5939,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU4" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="5" customFormat="1" s="7">
       <c r="A5" s="7" t="inlineStr">
@@ -6142,6 +6176,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="6" customFormat="1" s="7">
       <c r="A6" s="7" t="inlineStr">
@@ -6374,6 +6413,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU6" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="7" customFormat="1" s="7">
       <c r="A7" s="7" t="inlineStr">
@@ -6606,6 +6650,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU7" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="8" customFormat="1" s="7">
       <c r="A8" s="7" t="inlineStr">
@@ -6838,6 +6887,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="9" customFormat="1" s="7">
       <c r="A9" s="7" t="inlineStr">
@@ -7070,6 +7124,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU9" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="10" customFormat="1" s="7">
       <c r="A10" s="7" t="inlineStr">
@@ -7302,6 +7361,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="inlineStr">
@@ -7534,6 +7598,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU11" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="7" t="inlineStr">
@@ -7766,6 +7835,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU12" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="7" t="inlineStr">
@@ -7998,6 +8072,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="7" t="inlineStr">
@@ -8230,7 +8309,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AU14" s="7" t="n"/>
+      <c r="AU14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="AV14" s="7" t="n"/>
       <c r="AW14" s="7" t="n"/>
       <c r="AX14" s="7" t="n"/>
@@ -8477,6 +8560,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU15" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="7" t="inlineStr">
@@ -8709,6 +8797,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU16" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="7" t="inlineStr">
@@ -8743,17 +8836,17 @@
       </c>
       <c r="G17" s="1" t="inlineStr">
         <is>
-          <t>SAPCRE01_09102019084529JUK</t>
+          <t>SAPCRE01_17092020120338XPU</t>
         </is>
       </c>
       <c r="H17" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_09102019084825BWI</t>
+          <t>FACILITY-A_17092020121428</t>
         </is>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_09102019093813XDX</t>
+          <t>FACILITY-A_17092020142803SRE</t>
         </is>
       </c>
       <c r="J17" s="15" t="inlineStr">
@@ -8888,7 +8981,7 @@
       </c>
       <c r="AJ17" s="1" t="inlineStr">
         <is>
-          <t>Amendment Released No. U4130</t>
+          <t>Amendment Released No. U3116</t>
         </is>
       </c>
       <c r="AK17" s="5" t="inlineStr">
@@ -8939,6 +9032,11 @@
       <c r="AT17" s="5" t="inlineStr">
         <is>
           <t>-</t>
+        </is>
+      </c>
+      <c r="AU17" s="5" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -9173,6 +9271,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="inlineStr">
@@ -9405,6 +9508,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="7" t="inlineStr">
@@ -9439,17 +9547,17 @@
       </c>
       <c r="G20" s="1" t="inlineStr">
         <is>
-          <t>SAPCRE01_10102019150426QEP</t>
+          <t>SAPCRE01_17092020080016HFX</t>
         </is>
       </c>
       <c r="H20" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_10102019150724YCL</t>
+          <t>FACILITY-A_17092020080941</t>
         </is>
       </c>
       <c r="I20" s="32" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-17092020083654QDY</t>
         </is>
       </c>
       <c r="J20" s="14" t="inlineStr">
@@ -9627,6 +9735,11 @@
         </is>
       </c>
       <c r="AT20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AU20" s="5" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -9861,6 +9974,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU21" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="inlineStr">
@@ -10093,6 +10211,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU22" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="7" t="inlineStr">
@@ -10323,6 +10446,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU23" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -10555,6 +10683,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU24" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -10787,6 +10920,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU25" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -11019,6 +11157,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU26" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -11251,6 +11394,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU27" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="32" t="inlineStr">
@@ -11483,6 +11631,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU28" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="32" t="inlineStr">
@@ -11715,6 +11868,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU29" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="32" t="inlineStr">
@@ -11945,6 +12103,11 @@
           <t>Pri</t>
         </is>
       </c>
+      <c r="AU30" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="32" t="inlineStr">
@@ -12177,6 +12340,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU31" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="32" t="inlineStr">
@@ -12409,6 +12577,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="AU32" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="32" t="inlineStr">
@@ -12634,6 +12807,11 @@
       <c r="AS33" s="26" t="inlineStr">
         <is>
           <t>Y</t>
+        </is>
+      </c>
+      <c r="AU33" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -12747,7 +12925,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_16092020115532</t>
+          <t>FACILITY-A_17092020121428</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -13741,9 +13919,9 @@
   </sheetPr>
   <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -13922,7 +14100,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FACILITY-A_16092020115532</t>
+          <t>FACILITY-A_17092020121428</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -13932,7 +14110,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3000684</t>
+          <t>3000703</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -13965,7 +14143,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q2" s="32" t="n"/>
+      <c r="Q2" s="32" t="inlineStr"/>
       <c r="R2" s="1" t="inlineStr">
         <is>
           <t>user</t>
@@ -13973,7 +14151,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>-$EGLNUO</t>
+          <t>GWEGNKTE</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
@@ -14740,7 +14918,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q11" s="32" t="inlineStr"/>
+      <c r="Q11" s="32" t="n"/>
       <c r="R11" s="1" t="inlineStr">
         <is>
           <t>user</t>
@@ -14917,7 +15095,7 @@
       </c>
       <c r="H13" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_09102019093813XDX</t>
+          <t>FACILITY-A_17092020142803SRE</t>
         </is>
       </c>
       <c r="I13" s="1" t="inlineStr">
@@ -14927,7 +15105,7 @@
       </c>
       <c r="J13" s="1" t="inlineStr">
         <is>
-          <t>3000042</t>
+          <t>3000706</t>
         </is>
       </c>
       <c r="K13" s="1" t="inlineStr">
@@ -14942,7 +15120,12 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Borrower/true/5;Payload_effectiveDate;30-Nov-2018</t>
+          <t>Borrower/true/6</t>
+        </is>
+      </c>
+      <c r="N13" s="39" t="inlineStr">
+        <is>
+          <t>2020-11-23</t>
         </is>
       </c>
       <c r="O13" s="1" t="inlineStr">
@@ -14955,11 +15138,7 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q13" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="Q13" s="32" t="inlineStr"/>
       <c r="R13" s="1" t="inlineStr">
         <is>
           <t>user</t>
@@ -14967,12 +15146,12 @@
       </c>
       <c r="S13" s="1" t="inlineStr">
         <is>
-          <t>+HDYYDV2</t>
+          <t>0@EGNPJ3</t>
         </is>
       </c>
       <c r="T13" s="1" t="inlineStr">
         <is>
-          <t>HSSUPR01</t>
+          <t>SUPDEL01</t>
         </is>
       </c>
       <c r="U13" s="1" t="inlineStr">
@@ -15022,36 +15201,6 @@
           <t>Update</t>
         </is>
       </c>
-      <c r="H14" s="1" t="inlineStr">
-        <is>
-          <t>FACILITY-A_10102019150724YCL</t>
-        </is>
-      </c>
-      <c r="I14" s="1" t="inlineStr">
-        <is>
-          <t>TAM</t>
-        </is>
-      </c>
-      <c r="J14" s="1" t="inlineStr">
-        <is>
-          <t>3000062</t>
-        </is>
-      </c>
-      <c r="K14" s="1" t="inlineStr">
-        <is>
-          <t>CB001</t>
-        </is>
-      </c>
-      <c r="L14" s="1" t="inlineStr">
-        <is>
-          <t>AUSAG</t>
-        </is>
-      </c>
-      <c r="M14" s="1" t="inlineStr">
-        <is>
-          <t>Borrower/true/6</t>
-        </is>
-      </c>
       <c r="N14" s="1" t="inlineStr">
         <is>
           <t>2018-03-05</t>
@@ -15067,34 +15216,15 @@
           <t>true</t>
         </is>
       </c>
-      <c r="Q14" s="32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="Q14" s="32" t="n"/>
       <c r="R14" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
       </c>
-      <c r="S14" s="1" t="inlineStr">
-        <is>
-          <t>O6DZ0NBQ</t>
-        </is>
-      </c>
-      <c r="T14" s="1" t="inlineStr">
-        <is>
-          <t>HSSUPR01</t>
-        </is>
-      </c>
       <c r="U14" s="1" t="inlineStr">
         <is>
           <t>Facility Change Transaction Released</t>
-        </is>
-      </c>
-      <c r="V14" s="1" t="inlineStr">
-        <is>
-          <t>ZONE3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GDE-6969 removed comments and log
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/SAPWUL/SAPWUL_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/SAPWUL/SAPWUL_Data_Set.xlsx
@@ -1007,12 +1007,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SAPCRE01_17092020120338XPU</t>
+          <t>SAPCRE01_17092020160113UPY</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>D1_17092020120341RAL</t>
+          <t>D1_17092020160115UDD</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -5267,12 +5267,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SAPCRE01_17092020120338XPU</t>
+          <t>SAPCRE01_17092020160113UPY</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FACILITY-A_17092020121428</t>
+          <t>FACILITY-A_17092020161137</t>
         </is>
       </c>
       <c r="I2" s="32" t="inlineStr">
@@ -8836,17 +8836,17 @@
       </c>
       <c r="G17" s="1" t="inlineStr">
         <is>
-          <t>SAPCRE01_17092020120338XPU</t>
+          <t>SAPCRE01_17092020160113UPY</t>
         </is>
       </c>
       <c r="H17" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_17092020121428</t>
+          <t>FACILITY-A_17092020161137</t>
         </is>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_17092020142803SRE</t>
+          <t>FACILITY-A_17092020173354KAP</t>
         </is>
       </c>
       <c r="J17" s="15" t="inlineStr">
@@ -8981,7 +8981,7 @@
       </c>
       <c r="AJ17" s="1" t="inlineStr">
         <is>
-          <t>Amendment Released No. U3116</t>
+          <t>Amendment Released No. U3706</t>
         </is>
       </c>
       <c r="AK17" s="5" t="inlineStr">
@@ -12925,7 +12925,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_17092020121428</t>
+          <t>FACILITY-A_17092020161137</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -14100,7 +14100,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FACILITY-A_17092020121428</t>
+          <t>FACILITY-A_17092020161137</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -14110,7 +14110,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3000703</t>
+          <t>3000709</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -14151,7 +14151,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>GWEGNKTE</t>
+          <t>+0EGNUCV</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
@@ -15095,7 +15095,7 @@
       </c>
       <c r="H13" s="1" t="inlineStr">
         <is>
-          <t>FACILITY-A_17092020142803SRE</t>
+          <t>FACILITY-A_17092020173354KAP</t>
         </is>
       </c>
       <c r="I13" s="1" t="inlineStr">
@@ -15105,7 +15105,7 @@
       </c>
       <c r="J13" s="1" t="inlineStr">
         <is>
-          <t>3000706</t>
+          <t>3000711</t>
         </is>
       </c>
       <c r="K13" s="1" t="inlineStr">
@@ -15125,7 +15125,7 @@
       </c>
       <c r="N13" s="39" t="inlineStr">
         <is>
-          <t>2020-11-23</t>
+          <t>2020-11-24</t>
         </is>
       </c>
       <c r="O13" s="1" t="inlineStr">
@@ -15146,7 +15146,7 @@
       </c>
       <c r="S13" s="1" t="inlineStr">
         <is>
-          <t>0@EGNPJ3</t>
+          <t>AOEGNY4V</t>
         </is>
       </c>
       <c r="T13" s="1" t="inlineStr">

</xml_diff>